<commit_message>
Fixed Pandas Warning and adapted cmd-line output and menue
</commit_message>
<xml_diff>
--- a/Manual Tasks/ZLG_Testdaten_MAPPING.xlsx
+++ b/Manual Tasks/ZLG_Testdaten_MAPPING.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\richter122\git-projects\openehr_flat_loader\Manual Tasks\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
@@ -10,12 +15,12 @@
     <sheet name="Mapping CSV2openEHR" sheetId="1" r:id="rId1"/>
     <sheet name="FLAT_Paths" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="49">
   <si>
     <t>FLAT-Path</t>
   </si>
@@ -167,8 +172,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -201,15 +206,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -251,7 +264,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -283,9 +296,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -317,6 +331,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -492,19 +507,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="50.7109375" customWidth="1"/>
     <col min="2" max="2" width="80.7109375" customWidth="1"/>
     <col min="4" max="4" width="30.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>28</v>
       </c>
@@ -518,7 +535,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>33</v>
       </c>
@@ -526,7 +543,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>34</v>
       </c>
@@ -534,278 +551,336 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="8" spans="1:4">
+      <c r="B7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="17" spans="1:1">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>48</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="16">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2">
-      <formula1>FLAT_Paths!$A$2:$A$28</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3">
-      <formula1>FLAT_Paths!$A$2:$A$28</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4">
-      <formula1>FLAT_Paths!$A$2:$A$28</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5">
-      <formula1>FLAT_Paths!$A$2:$A$28</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6">
-      <formula1>FLAT_Paths!$A$2:$A$28</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B7">
-      <formula1>FLAT_Paths!$A$2:$A$28</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B8">
-      <formula1>FLAT_Paths!$A$2:$A$28</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B9">
-      <formula1>FLAT_Paths!$A$2:$A$28</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B10">
-      <formula1>FLAT_Paths!$A$2:$A$28</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B11">
-      <formula1>FLAT_Paths!$A$2:$A$28</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B12">
-      <formula1>FLAT_Paths!$A$2:$A$28</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B13">
-      <formula1>FLAT_Paths!$A$2:$A$28</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B14">
-      <formula1>FLAT_Paths!$A$2:$A$28</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B15">
-      <formula1>FLAT_Paths!$A$2:$A$28</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B16">
-      <formula1>FLAT_Paths!$A$2:$A$28</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B17">
-      <formula1>FLAT_Paths!$A$2:$A$28</formula1>
-    </dataValidation>
-  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="16">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>FLAT_Paths!$A$2:$A$28</xm:f>
+          </x14:formula1>
+          <xm:sqref>B2</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>FLAT_Paths!$A$2:$A$28</xm:f>
+          </x14:formula1>
+          <xm:sqref>B3</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>FLAT_Paths!$A$2:$A$28</xm:f>
+          </x14:formula1>
+          <xm:sqref>B4</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>FLAT_Paths!$A$2:$A$28</xm:f>
+          </x14:formula1>
+          <xm:sqref>B5</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>FLAT_Paths!$A$2:$A$28</xm:f>
+          </x14:formula1>
+          <xm:sqref>B6</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>FLAT_Paths!$A$2:$A$28</xm:f>
+          </x14:formula1>
+          <xm:sqref>B7</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>FLAT_Paths!$A$2:$A$28</xm:f>
+          </x14:formula1>
+          <xm:sqref>B8</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>FLAT_Paths!$A$2:$A$28</xm:f>
+          </x14:formula1>
+          <xm:sqref>B9</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>FLAT_Paths!$A$2:$A$28</xm:f>
+          </x14:formula1>
+          <xm:sqref>B10</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>FLAT_Paths!$A$2:$A$28</xm:f>
+          </x14:formula1>
+          <xm:sqref>B11</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>FLAT_Paths!$A$2:$A$28</xm:f>
+          </x14:formula1>
+          <xm:sqref>B12</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>FLAT_Paths!$A$2:$A$28</xm:f>
+          </x14:formula1>
+          <xm:sqref>B13</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>FLAT_Paths!$A$2:$A$28</xm:f>
+          </x14:formula1>
+          <xm:sqref>B14</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>FLAT_Paths!$A$2:$A$28</xm:f>
+          </x14:formula1>
+          <xm:sqref>B15</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>FLAT_Paths!$A$2:$A$28</xm:f>
+          </x14:formula1>
+          <xm:sqref>B16</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>FLAT_Paths!$A$2:$A$28</xm:f>
+          </x14:formula1>
+          <xm:sqref>B17</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A28"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="50.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:1">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:1">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:1">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:1">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:1">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:1">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:1">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:1">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:1">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:1">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:1">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:1">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:1">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:1">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:1">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:1">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:1">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:1">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:1">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:1">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:1">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:1">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:1">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:1">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:1">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>27</v>
       </c>

</xml_diff>

<commit_message>
Adapted WebPage and stored auth info as base64-encoding in config
</commit_message>
<xml_diff>
--- a/Manual Tasks/ZLG_Testdaten_MAPPING.xlsx
+++ b/Manual Tasks/ZLG_Testdaten_MAPPING.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\richter122\git-projects\openehr_flat_loader\Manual Tasks\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
@@ -15,12 +10,12 @@
     <sheet name="Mapping CSV2openEHR" sheetId="1" r:id="rId1"/>
     <sheet name="FLAT_Paths" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="49">
   <si>
     <t>FLAT-Path</t>
   </si>
@@ -172,8 +167,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -206,23 +201,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -264,7 +251,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -296,10 +283,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -331,7 +317,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -507,21 +492,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="50.7109375" customWidth="1"/>
     <col min="2" max="2" width="80.7109375" customWidth="1"/>
     <col min="4" max="4" width="30.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>28</v>
       </c>
@@ -535,7 +518,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>33</v>
       </c>
@@ -543,7 +526,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>34</v>
       </c>
@@ -551,336 +534,278 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4">
       <c r="A5" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4">
       <c r="A6" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4">
       <c r="A7" t="s">
         <v>38</v>
       </c>
-      <c r="B7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:4">
       <c r="A8" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4">
       <c r="A9" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4">
       <c r="A10" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4">
       <c r="A11" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4">
       <c r="A12" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4">
       <c r="A13" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4">
       <c r="A14" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4">
       <c r="A15" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4">
       <c r="A16" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1">
       <c r="A17" t="s">
         <v>48</v>
       </c>
     </row>
   </sheetData>
+  <dataValidations count="16">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2">
+      <formula1>FLAT_Paths!$A$2:$A$28</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3">
+      <formula1>FLAT_Paths!$A$2:$A$28</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4">
+      <formula1>FLAT_Paths!$A$2:$A$28</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5">
+      <formula1>FLAT_Paths!$A$2:$A$28</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6">
+      <formula1>FLAT_Paths!$A$2:$A$28</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B7">
+      <formula1>FLAT_Paths!$A$2:$A$28</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B8">
+      <formula1>FLAT_Paths!$A$2:$A$28</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B9">
+      <formula1>FLAT_Paths!$A$2:$A$28</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B10">
+      <formula1>FLAT_Paths!$A$2:$A$28</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B11">
+      <formula1>FLAT_Paths!$A$2:$A$28</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B12">
+      <formula1>FLAT_Paths!$A$2:$A$28</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B13">
+      <formula1>FLAT_Paths!$A$2:$A$28</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B14">
+      <formula1>FLAT_Paths!$A$2:$A$28</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B15">
+      <formula1>FLAT_Paths!$A$2:$A$28</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B16">
+      <formula1>FLAT_Paths!$A$2:$A$28</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B17">
+      <formula1>FLAT_Paths!$A$2:$A$28</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="16">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>FLAT_Paths!$A$2:$A$28</xm:f>
-          </x14:formula1>
-          <xm:sqref>B2</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>FLAT_Paths!$A$2:$A$28</xm:f>
-          </x14:formula1>
-          <xm:sqref>B3</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>FLAT_Paths!$A$2:$A$28</xm:f>
-          </x14:formula1>
-          <xm:sqref>B4</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>FLAT_Paths!$A$2:$A$28</xm:f>
-          </x14:formula1>
-          <xm:sqref>B5</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>FLAT_Paths!$A$2:$A$28</xm:f>
-          </x14:formula1>
-          <xm:sqref>B6</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>FLAT_Paths!$A$2:$A$28</xm:f>
-          </x14:formula1>
-          <xm:sqref>B7</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>FLAT_Paths!$A$2:$A$28</xm:f>
-          </x14:formula1>
-          <xm:sqref>B8</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>FLAT_Paths!$A$2:$A$28</xm:f>
-          </x14:formula1>
-          <xm:sqref>B9</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>FLAT_Paths!$A$2:$A$28</xm:f>
-          </x14:formula1>
-          <xm:sqref>B10</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>FLAT_Paths!$A$2:$A$28</xm:f>
-          </x14:formula1>
-          <xm:sqref>B11</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>FLAT_Paths!$A$2:$A$28</xm:f>
-          </x14:formula1>
-          <xm:sqref>B12</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>FLAT_Paths!$A$2:$A$28</xm:f>
-          </x14:formula1>
-          <xm:sqref>B13</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>FLAT_Paths!$A$2:$A$28</xm:f>
-          </x14:formula1>
-          <xm:sqref>B14</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>FLAT_Paths!$A$2:$A$28</xm:f>
-          </x14:formula1>
-          <xm:sqref>B15</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>FLAT_Paths!$A$2:$A$28</xm:f>
-          </x14:formula1>
-          <xm:sqref>B16</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>FLAT_Paths!$A$2:$A$28</xm:f>
-          </x14:formula1>
-          <xm:sqref>B17</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:A28"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="50.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1">
       <c r="A3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1">
       <c r="A4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1">
       <c r="A5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1">
       <c r="A6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1">
       <c r="A7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1">
       <c r="A8" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1">
       <c r="A9" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:1">
       <c r="A10" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:1">
       <c r="A11" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:1">
       <c r="A12" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:1">
       <c r="A13" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:1">
       <c r="A14" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:1">
       <c r="A15" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:1">
       <c r="A16" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1">
       <c r="A17" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1">
       <c r="A18" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1">
       <c r="A19" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1">
       <c r="A20" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1">
       <c r="A21" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1">
       <c r="A22" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1">
       <c r="A23" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1">
       <c r="A24" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1">
       <c r="A25" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:1">
       <c r="A26" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:1">
       <c r="A27" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:1">
       <c r="A28" t="s">
         <v>27</v>
       </c>

</xml_diff>

<commit_message>
Changed Input Dir Structure. Fixed Redirecting to correct tab panel after uploading a file. Tested dynamic rendering in html with flask variables.
</commit_message>
<xml_diff>
--- a/Manual Tasks/ZLG_Testdaten_MAPPING.xlsx
+++ b/Manual Tasks/ZLG_Testdaten_MAPPING.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\richter122\git-projects\openehr_flat_loader\Manual Tasks\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
@@ -10,12 +15,12 @@
     <sheet name="Mapping CSV2openEHR" sheetId="1" r:id="rId1"/>
     <sheet name="FLAT_Paths" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="49">
   <si>
     <t>FLAT-Path</t>
   </si>
@@ -167,8 +172,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -201,15 +206,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -251,7 +264,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -283,9 +296,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -317,6 +331,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -492,19 +507,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="50.7109375" customWidth="1"/>
     <col min="2" max="2" width="80.7109375" customWidth="1"/>
     <col min="4" max="4" width="30.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>28</v>
       </c>
@@ -518,7 +535,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>33</v>
       </c>
@@ -526,7 +543,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>34</v>
       </c>
@@ -534,278 +551,333 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="6" spans="1:4">
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="17" spans="1:1">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>48</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="16">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2">
-      <formula1>FLAT_Paths!$A$2:$A$28</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3">
-      <formula1>FLAT_Paths!$A$2:$A$28</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4">
-      <formula1>FLAT_Paths!$A$2:$A$28</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5">
-      <formula1>FLAT_Paths!$A$2:$A$28</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6">
-      <formula1>FLAT_Paths!$A$2:$A$28</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B7">
-      <formula1>FLAT_Paths!$A$2:$A$28</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B8">
-      <formula1>FLAT_Paths!$A$2:$A$28</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B9">
-      <formula1>FLAT_Paths!$A$2:$A$28</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B10">
-      <formula1>FLAT_Paths!$A$2:$A$28</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B11">
-      <formula1>FLAT_Paths!$A$2:$A$28</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B12">
-      <formula1>FLAT_Paths!$A$2:$A$28</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B13">
-      <formula1>FLAT_Paths!$A$2:$A$28</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B14">
-      <formula1>FLAT_Paths!$A$2:$A$28</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B15">
-      <formula1>FLAT_Paths!$A$2:$A$28</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B16">
-      <formula1>FLAT_Paths!$A$2:$A$28</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B17">
-      <formula1>FLAT_Paths!$A$2:$A$28</formula1>
-    </dataValidation>
-  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="16">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>FLAT_Paths!$A$2:$A$28</xm:f>
+          </x14:formula1>
+          <xm:sqref>B2</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>FLAT_Paths!$A$2:$A$28</xm:f>
+          </x14:formula1>
+          <xm:sqref>B3</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>FLAT_Paths!$A$2:$A$28</xm:f>
+          </x14:formula1>
+          <xm:sqref>B4</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>FLAT_Paths!$A$2:$A$28</xm:f>
+          </x14:formula1>
+          <xm:sqref>B5</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>FLAT_Paths!$A$2:$A$28</xm:f>
+          </x14:formula1>
+          <xm:sqref>B6</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>FLAT_Paths!$A$2:$A$28</xm:f>
+          </x14:formula1>
+          <xm:sqref>B7</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>FLAT_Paths!$A$2:$A$28</xm:f>
+          </x14:formula1>
+          <xm:sqref>B8</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>FLAT_Paths!$A$2:$A$28</xm:f>
+          </x14:formula1>
+          <xm:sqref>B9</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>FLAT_Paths!$A$2:$A$28</xm:f>
+          </x14:formula1>
+          <xm:sqref>B10</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>FLAT_Paths!$A$2:$A$28</xm:f>
+          </x14:formula1>
+          <xm:sqref>B11</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>FLAT_Paths!$A$2:$A$28</xm:f>
+          </x14:formula1>
+          <xm:sqref>B12</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>FLAT_Paths!$A$2:$A$28</xm:f>
+          </x14:formula1>
+          <xm:sqref>B13</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>FLAT_Paths!$A$2:$A$28</xm:f>
+          </x14:formula1>
+          <xm:sqref>B14</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>FLAT_Paths!$A$2:$A$28</xm:f>
+          </x14:formula1>
+          <xm:sqref>B15</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>FLAT_Paths!$A$2:$A$28</xm:f>
+          </x14:formula1>
+          <xm:sqref>B16</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>FLAT_Paths!$A$2:$A$28</xm:f>
+          </x14:formula1>
+          <xm:sqref>B17</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A28"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="50.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:1">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:1">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:1">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:1">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:1">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:1">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:1">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:1">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:1">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:1">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:1">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:1">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:1">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:1">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:1">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:1">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:1">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:1">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:1">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:1">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:1">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:1">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:1">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:1">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:1">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>27</v>
       </c>

</xml_diff>